<commit_message>
[sanket] - minor changes
</commit_message>
<xml_diff>
--- a/utility-service/assets/testing_excel.xlsx
+++ b/utility-service/assets/testing_excel.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sanket Agrawal\Learning\email-sender\utility-service\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A752E1-8632-433A-BEC5-7BC7468BD5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA82292-EDF4-4D17-B5B5-07D0C2E42A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6C29F34F-1FAA-4DB0-A0FA-39123FDF88E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Email" sheetId="2" r:id="rId1"/>
-    <sheet name="Hello" sheetId="3" r:id="rId2"/>
+    <sheet name="Backup-Sheet" sheetId="4" r:id="rId2"/>
+    <sheet name="Hello" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="121">
   <si>
     <t>Company</t>
   </si>
@@ -45,16 +46,361 @@
     <t>Email</t>
   </si>
   <si>
-    <t>sanket@ataloud.com</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
     <t>Position</t>
   </si>
   <si>
-    <t>thesanketagrawal@gmail.com</t>
+    <t>careers@sensehawk.com</t>
+  </si>
+  <si>
+    <t>bsireesha@teksystems.com</t>
+  </si>
+  <si>
+    <t>apshetty@astoncarter.com</t>
+  </si>
+  <si>
+    <t>vsputtapaka@adaequare.com</t>
+  </si>
+  <si>
+    <t>jyothip@aapmor.com</t>
+  </si>
+  <si>
+    <t>Rahul.Raj6@Techmahindra.com</t>
+  </si>
+  <si>
+    <t>megha@jigsawinc.in</t>
+  </si>
+  <si>
+    <t>komal.gutti@automationedge.com</t>
+  </si>
+  <si>
+    <t>Cody@clutchnow.com</t>
+  </si>
+  <si>
+    <t>shruti.phatale@martlenz.com</t>
+  </si>
+  <si>
+    <t>mj00642401@techmahindra.com</t>
+  </si>
+  <si>
+    <t>Krupa_jugade@persistent.com</t>
+  </si>
+  <si>
+    <t>vaibhav.shah@canopusinfosystems.com</t>
+  </si>
+  <si>
+    <t>jobs@triangleglobal.com</t>
+  </si>
+  <si>
+    <t>pranali.p@boyenhaddin.com</t>
+  </si>
+  <si>
+    <t>janhavig@godrej.com</t>
+  </si>
+  <si>
+    <t>umar@nexionpro.com</t>
+  </si>
+  <si>
+    <t>hrd.sipcot@shardamotor.com</t>
+  </si>
+  <si>
+    <t>moinul.hasan@bengalmobileqa.com</t>
+  </si>
+  <si>
+    <t>satish.b@twsol.com</t>
+  </si>
+  <si>
+    <t>gurmeet.singh@alfanar.com</t>
+  </si>
+  <si>
+    <t>jobs@trellissoft.ai</t>
+  </si>
+  <si>
+    <t>hr@nexushire.in</t>
+  </si>
+  <si>
+    <t>ektanarula@aquissearch.com</t>
+  </si>
+  <si>
+    <t>sanjays@teamworks.org.in</t>
+  </si>
+  <si>
+    <t>priyankas@newtglobalcorp.com</t>
+  </si>
+  <si>
+    <t>ridham@richestsoft.in</t>
+  </si>
+  <si>
+    <t>sauravs@cleanhydrogentechnologies.com</t>
+  </si>
+  <si>
+    <t>srikrishna.jogi@spoors.in</t>
+  </si>
+  <si>
+    <t>mary.soliman@collaberadigital.com</t>
+  </si>
+  <si>
+    <t>hr@thefabcode.org</t>
+  </si>
+  <si>
+    <t>krishna@escanav.com</t>
+  </si>
+  <si>
+    <t>chaitalimali@sumagoinfotech.in</t>
+  </si>
+  <si>
+    <t>nikita.panchal@kaseya.com</t>
+  </si>
+  <si>
+    <t>info@shjintl.com</t>
+  </si>
+  <si>
+    <t>hr@nenosystems.com</t>
+  </si>
+  <si>
+    <t>Milind.lalcheta@productsquads.com</t>
+  </si>
+  <si>
+    <t>career@clarigoinfotech.com</t>
+  </si>
+  <si>
+    <t>hr@blueweaveconsulting.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hardik@blueweaveconsulting.com </t>
+  </si>
+  <si>
+    <t>shalini@blueweaveconsulting.com</t>
+  </si>
+  <si>
+    <t>csharma@nownow.ng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sowmya.naidu@bpterp.com </t>
+  </si>
+  <si>
+    <t>sayaji@expediteinformatics.com</t>
+  </si>
+  <si>
+    <t>asthasingh@aquissearch.com</t>
+  </si>
+  <si>
+    <t>pushpalatha.bk@drivex.in</t>
+  </si>
+  <si>
+    <t>neha.chubby@belwo.com</t>
+  </si>
+  <si>
+    <t>payal.nagpal@in.ey.com</t>
+  </si>
+  <si>
+    <t>shivam.kandhari@igtsolutions.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">akshatha.gowda@neominds.in </t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Tek Systems</t>
+  </si>
+  <si>
+    <t>Aston Carter</t>
+  </si>
+  <si>
+    <t>Sireesha</t>
+  </si>
+  <si>
+    <t>Sir</t>
+  </si>
+  <si>
+    <t>Jyothi</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>Tech Mahindra</t>
+  </si>
+  <si>
+    <t>Jigsaw</t>
+  </si>
+  <si>
+    <t>Megha</t>
+  </si>
+  <si>
+    <t>Cody</t>
+  </si>
+  <si>
+    <t>Umar</t>
+  </si>
+  <si>
+    <t>Ridham</t>
+  </si>
+  <si>
+    <t>Krishna</t>
+  </si>
+  <si>
+    <t>Hardik</t>
+  </si>
+  <si>
+    <t>Shalini</t>
+  </si>
+  <si>
+    <t>Csharma</t>
+  </si>
+  <si>
+    <t>Sayaji</t>
+  </si>
+  <si>
+    <t>Komal</t>
+  </si>
+  <si>
+    <t>Automation Edge</t>
+  </si>
+  <si>
+    <t>Shruti</t>
+  </si>
+  <si>
+    <t>Krupa</t>
+  </si>
+  <si>
+    <t>Vaibhav</t>
+  </si>
+  <si>
+    <t>Pranali</t>
+  </si>
+  <si>
+    <t>Moinul</t>
+  </si>
+  <si>
+    <t>Satish</t>
+  </si>
+  <si>
+    <t>Gurmeet</t>
+  </si>
+  <si>
+    <t>Persistent</t>
+  </si>
+  <si>
+    <t>Godrej</t>
+  </si>
+  <si>
+    <t>Canopus</t>
+  </si>
+  <si>
+    <t>Janhavi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nexion </t>
+  </si>
+  <si>
+    <t>Sharda Motor</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Nikita</t>
+  </si>
+  <si>
+    <t>Ekta</t>
+  </si>
+  <si>
+    <t>Aquis Search</t>
+  </si>
+  <si>
+    <t>Sanjay</t>
+  </si>
+  <si>
+    <t>Saurav</t>
+  </si>
+  <si>
+    <t>Milind</t>
+  </si>
+  <si>
+    <t>Akshat</t>
+  </si>
+  <si>
+    <t>Sowmya</t>
+  </si>
+  <si>
+    <t>Pushpa</t>
+  </si>
+  <si>
+    <t>Shivam</t>
+  </si>
+  <si>
+    <t>Priyanka</t>
+  </si>
+  <si>
+    <t>Chaitali</t>
+  </si>
+  <si>
+    <t>Astha</t>
+  </si>
+  <si>
+    <t>Neha</t>
+  </si>
+  <si>
+    <t>Payal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Richest </t>
+  </si>
+  <si>
+    <t>Nownow</t>
+  </si>
+  <si>
+    <t>Spoors</t>
+  </si>
+  <si>
+    <t>Thefabcode</t>
+  </si>
+  <si>
+    <t>Escanav</t>
+  </si>
+  <si>
+    <t>Kaseya</t>
+  </si>
+  <si>
+    <t>Productsquads</t>
+  </si>
+  <si>
+    <t>Neominds</t>
+  </si>
+  <si>
+    <t>Drivex</t>
+  </si>
+  <si>
+    <t>Belwo</t>
+  </si>
+  <si>
+    <t>Collabera Digital</t>
+  </si>
+  <si>
+    <t>Sumago Infotech</t>
+  </si>
+  <si>
+    <t>Shji</t>
+  </si>
+  <si>
+    <t>Neno Systems</t>
+  </si>
+  <si>
+    <t>Clarigo Infotech</t>
+  </si>
+  <si>
+    <t>Expedite Informatics</t>
+  </si>
+  <si>
+    <t>EY</t>
+  </si>
+  <si>
+    <t>Igt Solutions</t>
   </si>
 </sst>
 </file>
@@ -417,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8444E725-B3FA-46FD-8FF2-B3261EAC90FF}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,7 +778,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -441,62 +787,533 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C2" s="1" t="s">
-        <v>2</v>
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C3" s="1" t="s">
-        <v>5</v>
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C4" s="1"/>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C5" s="1"/>
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C6" s="1"/>
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C7" s="1"/>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C8" s="1"/>
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C9" s="1"/>
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C10" s="1"/>
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C11" s="1"/>
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>116</v>
+      </c>
+      <c r="C29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>100</v>
+      </c>
+      <c r="B39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>96</v>
+      </c>
+      <c r="B40" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>102</v>
+      </c>
+      <c r="B42" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{DFDD7DDD-3D64-4103-B4B0-51FE258E1EAA}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{6111CB2F-01AA-4A6B-9915-BAB05E0781B2}"/>
+    <hyperlink ref="C35" r:id="rId1" xr:uid="{5C1CFA74-5BC4-4C7C-9111-0C9FF38B4DF5}"/>
+    <hyperlink ref="C43" r:id="rId2" xr:uid="{C5ECE9A3-5F85-41D7-BFFB-741518D365E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A146E0-6AEF-4390-BD33-8DDA3761DD15}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6936211C-D653-4A97-BE72-80C0A42448D0}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A146E0-6AEF-4390-BD33-8DDA3761DD15}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:C46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>6362993319</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>